<commit_message>
chore: added data to categories
</commit_message>
<xml_diff>
--- a/categorias_definicoes.xlsx
+++ b/categorias_definicoes.xlsx
@@ -4,39 +4,254 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="108" windowWidth="22980" windowHeight="9288" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="108" windowWidth="22980" windowHeight="9288"/>
   </bookViews>
   <sheets>
     <sheet name="Inter_receitas" sheetId="1" r:id="rId1"/>
     <sheet name="Inter_custos" sheetId="6" r:id="rId2"/>
-    <sheet name="Itau_receitas" sheetId="2" r:id="rId3"/>
-    <sheet name="Itau_custos" sheetId="7" r:id="rId4"/>
-    <sheet name="Carrefour_receitas" sheetId="3" r:id="rId5"/>
-    <sheet name="Carrefour_custos" sheetId="8" r:id="rId6"/>
-    <sheet name="Caixa_receitas" sheetId="4" r:id="rId7"/>
-    <sheet name="Caixa_custos" sheetId="9" r:id="rId8"/>
-    <sheet name="Bradesco_receitas" sheetId="5" r:id="rId9"/>
-    <sheet name="Bradesco_custos" sheetId="10" r:id="rId10"/>
+    <sheet name="Caixa_receitas" sheetId="4" r:id="rId3"/>
+    <sheet name="Caixa_custos" sheetId="9" r:id="rId4"/>
+    <sheet name="Bradesco_receitas" sheetId="5" r:id="rId5"/>
+    <sheet name="Bradesco_custos" sheetId="10" r:id="rId6"/>
+    <sheet name="Itau_receitas" sheetId="2" r:id="rId7"/>
+    <sheet name="Itau_custos" sheetId="7" r:id="rId8"/>
+    <sheet name="Carrefour_receitas" sheetId="3" r:id="rId9"/>
+    <sheet name="Carrefour_custos" sheetId="8" r:id="rId10"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="71">
   <si>
     <t>Salários e Rendimentos</t>
   </si>
   <si>
-    <t>Reembolsos e Reversões</t>
+    <t>Investimentos</t>
+  </si>
+  <si>
+    <t>rendimentos poup facil-depos a partir</t>
+  </si>
+  <si>
+    <t>transf saldo c/sal p/cc</t>
+  </si>
+  <si>
+    <t>Movimentações</t>
+  </si>
+  <si>
+    <t>transferencia pix rem: napoleao ribeiro silv</t>
+  </si>
+  <si>
+    <t>Outros créditos</t>
+  </si>
+  <si>
+    <t>transferencia pix rem: maria amelia mendes d</t>
+  </si>
+  <si>
+    <t>credito de salario</t>
+  </si>
+  <si>
+    <t>Moradia</t>
+  </si>
+  <si>
+    <t>transferencia pix des: kaue boretti de lana</t>
+  </si>
+  <si>
+    <t>pix qr code estatico des: napoleao ribeiro silv</t>
+  </si>
+  <si>
+    <t>pagto eletron cobranca financeira ita cbd s.a0000033</t>
+  </si>
+  <si>
+    <t>Educação</t>
+  </si>
+  <si>
+    <t>pix qr code dinamico des: caixa de cursos ltda. 21/101348092</t>
+  </si>
+  <si>
+    <t>Outros débitos</t>
+  </si>
+  <si>
+    <t>transferencia pix des: eduardo ribeiro silva 22/101600542</t>
+  </si>
+  <si>
+    <t>estorno de rendimentos * poup facil-depos a partir 4/5/120004135</t>
+  </si>
+  <si>
+    <t>Assinaturas</t>
+  </si>
+  <si>
+    <t>amazon kindle unltd</t>
+  </si>
+  <si>
+    <t>google duolingo</t>
+  </si>
+  <si>
+    <t>anuidade diferenci</t>
+  </si>
+  <si>
+    <t>casasba*casas bahi</t>
+  </si>
+  <si>
+    <t>pagto ficha compensacao</t>
+  </si>
+  <si>
+    <t>encargos de atraso</t>
+  </si>
+  <si>
+    <t>deb iof</t>
+  </si>
+  <si>
+    <t>deb juros</t>
+  </si>
+  <si>
+    <t>compra</t>
+  </si>
+  <si>
+    <t>Lazer</t>
+  </si>
+  <si>
+    <t>Loteria</t>
+  </si>
+  <si>
+    <t>ap loteria</t>
+  </si>
+  <si>
+    <t>db cx cap</t>
+  </si>
+  <si>
+    <t>envio pix</t>
+  </si>
+  <si>
+    <t>saldo dia</t>
+  </si>
+  <si>
+    <t>db t cesta</t>
+  </si>
+  <si>
+    <t>cred pix</t>
+  </si>
+  <si>
+    <t>pg luz/gas</t>
+  </si>
+  <si>
+    <t>saque lot</t>
+  </si>
+  <si>
+    <t>cp elo</t>
+  </si>
+  <si>
+    <t>pag fone</t>
+  </si>
+  <si>
+    <t>pag boleto</t>
+  </si>
+  <si>
+    <t>cred inss</t>
+  </si>
+  <si>
+    <t>cred ted</t>
+  </si>
+  <si>
+    <t>dep din ag</t>
+  </si>
+  <si>
+    <t>dp din lot</t>
+  </si>
+  <si>
+    <t>crf 3 spp pinheiros</t>
+  </si>
+  <si>
+    <t>academia sempre viva i,sao paulo</t>
+  </si>
+  <si>
+    <t>htm*cursoclpeihm,coronel fabr-</t>
+  </si>
+  <si>
+    <t>pg *ton garra de agu,sao paulo</t>
+  </si>
+  <si>
+    <t>assai atacadista,sao paulo</t>
+  </si>
+  <si>
+    <t>advocacia dgl,maringa</t>
+  </si>
+  <si>
+    <t>otica bom preco,sao paulo</t>
+  </si>
+  <si>
+    <t>crf 48 spg giovanni gronc</t>
+  </si>
+  <si>
+    <t>shekinah comercio de m, sao paulo</t>
+  </si>
+  <si>
+    <t>agpsapataria, sao paulo</t>
+  </si>
+  <si>
+    <t>maravilha carnes parqu, sao paulo</t>
+  </si>
+  <si>
+    <t>anuidade diferenciada</t>
+  </si>
+  <si>
+    <t>p&amp;f mat. construcao, sao paulo</t>
+  </si>
+  <si>
+    <t>fabrica de oculos,sao paulo</t>
+  </si>
+  <si>
+    <t>mercadocar, sao paulo</t>
+  </si>
+  <si>
+    <t>planta e saude, sao paulo</t>
+  </si>
+  <si>
+    <t>megafarma, sao paulo</t>
+  </si>
+  <si>
+    <t>duda gas, sao paulo</t>
+  </si>
+  <si>
+    <t>akki atacadista, sao paulo</t>
+  </si>
+  <si>
+    <t>assai atacadista, sao paulo</t>
+  </si>
+  <si>
+    <t>resgate:</t>
+  </si>
+  <si>
+    <t>pix recebido:</t>
+  </si>
+  <si>
+    <t>pagamento</t>
+  </si>
+  <si>
+    <t>credito evento b3:</t>
+  </si>
+  <si>
+    <t>aplicacao:</t>
+  </si>
+  <si>
+    <t>-tim s a</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -64,8 +279,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -367,18 +584,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -387,6 +622,415 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B6" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="32.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B6" s="1"/>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H10" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="45.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="56.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -398,132 +1042,72 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="20.109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="20.109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
 </file>
</xml_diff>